<commit_message>
add: students list completed
</commit_message>
<xml_diff>
--- a/studentList.xlsx
+++ b/studentList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>Nom</t>
   </si>
@@ -27,94 +27,274 @@
     <t>Prenom</t>
   </si>
   <si>
-    <t>eleve1</t>
-  </si>
-  <si>
-    <t>eleve2</t>
-  </si>
-  <si>
-    <t>eleve3</t>
-  </si>
-  <si>
-    <t>eleve4</t>
-  </si>
-  <si>
-    <t>eleve5</t>
-  </si>
-  <si>
-    <t>eleve6</t>
-  </si>
-  <si>
-    <t>eleve7</t>
-  </si>
-  <si>
-    <t>eleve8</t>
-  </si>
-  <si>
-    <t>eleve9</t>
-  </si>
-  <si>
-    <t>eleve10</t>
-  </si>
-  <si>
-    <t>eleve11</t>
-  </si>
-  <si>
-    <t>eleve12</t>
-  </si>
-  <si>
-    <t>eleve13</t>
-  </si>
-  <si>
-    <t>eleve14</t>
-  </si>
-  <si>
-    <t>eleve15</t>
-  </si>
-  <si>
-    <t>eleve16</t>
-  </si>
-  <si>
-    <t>eleve17</t>
-  </si>
-  <si>
-    <t>eleve18</t>
-  </si>
-  <si>
-    <t>eleve19</t>
-  </si>
-  <si>
-    <t>eleve20</t>
-  </si>
-  <si>
-    <t>eleve21</t>
-  </si>
-  <si>
-    <t>eleve22</t>
-  </si>
-  <si>
-    <t>eleve23</t>
-  </si>
-  <si>
-    <t>eleve24</t>
-  </si>
-  <si>
-    <t>eleve25</t>
-  </si>
-  <si>
-    <t>eleve26</t>
-  </si>
-  <si>
-    <t>eleve27</t>
-  </si>
-  <si>
-    <t>eleve28</t>
-  </si>
-  <si>
-    <t>eleve29</t>
-  </si>
-  <si>
-    <t>eleve30</t>
+    <t>Joris</t>
+  </si>
+  <si>
+    <t>Granel</t>
+  </si>
+  <si>
+    <t>Maxime</t>
+  </si>
+  <si>
+    <t>Soustelle</t>
+  </si>
+  <si>
+    <t>Lucie</t>
+  </si>
+  <si>
+    <t>Truong</t>
+  </si>
+  <si>
+    <t>Assil</t>
+  </si>
+  <si>
+    <t>El Yahyaoui</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Neplaz</t>
+  </si>
+  <si>
+    <t>Adrien</t>
+  </si>
+  <si>
+    <t>Roux</t>
+  </si>
+  <si>
+    <t>Johanna</t>
+  </si>
+  <si>
+    <t>Boiteux</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
+  </si>
+  <si>
+    <t>Bottero</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Maitre</t>
+  </si>
+  <si>
+    <t>Xeryus</t>
+  </si>
+  <si>
+    <t>Mauguy</t>
+  </si>
+  <si>
+    <t>Vincent</t>
+  </si>
+  <si>
+    <t>Herreros</t>
+  </si>
+  <si>
+    <t>Clément</t>
+  </si>
+  <si>
+    <t>Loubiere</t>
+  </si>
+  <si>
+    <t>Ophelie</t>
+  </si>
+  <si>
+    <t>Piekarek</t>
+  </si>
+  <si>
+    <t>Cyril</t>
+  </si>
+  <si>
+    <t>Pluche</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Aufauvre</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Giordani</t>
+  </si>
+  <si>
+    <t>Jade</t>
+  </si>
+  <si>
+    <t>Hennebert</t>
+  </si>
+  <si>
+    <t>Tristan</t>
+  </si>
+  <si>
+    <t>Riviere</t>
+  </si>
+  <si>
+    <t>Florent</t>
+  </si>
+  <si>
+    <t>Berland</t>
+  </si>
+  <si>
+    <t>Enzo</t>
+  </si>
+  <si>
+    <t>Fabre</t>
+  </si>
+  <si>
+    <t>Mohammed Ihe</t>
+  </si>
+  <si>
+    <t>Faiza</t>
+  </si>
+  <si>
+    <t>Marion</t>
+  </si>
+  <si>
+    <t>Rul</t>
+  </si>
+  <si>
+    <t>Antoine</t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Dalger</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Escalier</t>
+  </si>
+  <si>
+    <t>Toinon</t>
+  </si>
+  <si>
+    <t>Georget</t>
+  </si>
+  <si>
+    <t>Loris</t>
+  </si>
+  <si>
+    <t>Zirah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loic </t>
+  </si>
+  <si>
+    <t>Combis</t>
+  </si>
+  <si>
+    <t>Melvil</t>
+  </si>
+  <si>
+    <t>Donnart</t>
+  </si>
+  <si>
+    <t>Clement</t>
+  </si>
+  <si>
+    <t>Roig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Megane </t>
+  </si>
+  <si>
+    <t>Wintz</t>
+  </si>
+  <si>
+    <t>Remi</t>
+  </si>
+  <si>
+    <t>Bellicot</t>
+  </si>
+  <si>
+    <t>Achraf</t>
+  </si>
+  <si>
+    <t>El Mahmoudi</t>
+  </si>
+  <si>
+    <t>Illias</t>
+  </si>
+  <si>
+    <t>Mellah</t>
+  </si>
+  <si>
+    <t>Petit</t>
+  </si>
+  <si>
+    <t>Mahé</t>
+  </si>
+  <si>
+    <t>Spaenle</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Contremoulin</t>
+  </si>
+  <si>
+    <t>Hamelina</t>
+  </si>
+  <si>
+    <t>Ehamelo</t>
+  </si>
+  <si>
+    <t>Leclerc</t>
+  </si>
+  <si>
+    <t>Romain</t>
+  </si>
+  <si>
+    <t>Thevenon</t>
+  </si>
+  <si>
+    <t>Thais</t>
+  </si>
+  <si>
+    <t>Aurard</t>
+  </si>
+  <si>
+    <t>Amin</t>
+  </si>
+  <si>
+    <t>Bazaz</t>
+  </si>
+  <si>
+    <t>Matthieu</t>
+  </si>
+  <si>
+    <t>Dye</t>
+  </si>
+  <si>
+    <t>Cyprien</t>
+  </si>
+  <si>
+    <t>Legrand</t>
+  </si>
+  <si>
+    <t>Fabien</t>
+  </si>
+  <si>
+    <t>Turgut</t>
   </si>
 </sst>
 </file>
@@ -466,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,239 +667,367 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>